<commit_message>
Create study progress data
</commit_message>
<xml_diff>
--- a/BackEnd/src/Book1.xlsx
+++ b/BackEnd/src/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\BackEnd\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44713A60-C65A-4296-A295-FEB4F7D035E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD60EE35-E513-4675-A9E1-4C0D4B8D88F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1332" windowWidth="21000" windowHeight="10572" activeTab="1" xr2:uid="{FBC07B8B-4F86-43B9-A3CB-38C7923DBFA5}"/>
+    <workbookView xWindow="660" yWindow="1332" windowWidth="21000" windowHeight="10572" activeTab="2" xr2:uid="{FBC07B8B-4F86-43B9-A3CB-38C7923DBFA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ngành" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="287">
   <si>
     <t>Công nghệ thông tin</t>
   </si>
@@ -853,6 +853,54 @@
   </si>
   <si>
     <t>group_id</t>
+  </si>
+  <si>
+    <t>CN5</t>
+  </si>
+  <si>
+    <t>Công nghệ kỹ thuật xây dựng</t>
+  </si>
+  <si>
+    <t>Công nghệ kỹ thuật cơ điện tử</t>
+  </si>
+  <si>
+    <t>CN6</t>
+  </si>
+  <si>
+    <t>CN9</t>
+  </si>
+  <si>
+    <t>Công nghệ kỹ thuật điện tử – viễn thông</t>
+  </si>
+  <si>
+    <t>Công nghệ nông nghiệp</t>
+  </si>
+  <si>
+    <t>CN10</t>
+  </si>
+  <si>
+    <t>Kỹ thuật điều khiển và tự động hóa</t>
+  </si>
+  <si>
+    <t>CN11</t>
+  </si>
+  <si>
+    <t>Kỹ thuật năng lượng</t>
+  </si>
+  <si>
+    <t>CN13</t>
+  </si>
+  <si>
+    <t>Thiết kế công nghiệp và đồ họa</t>
+  </si>
+  <si>
+    <t>CN18</t>
+  </si>
+  <si>
+    <t>CN17</t>
+  </si>
+  <si>
+    <t>Kỹ thuật Robot</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDC965C-E5ED-4A6E-8BE3-35CB90B5606C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1370,6 +1418,70 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>280</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>282</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>284</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>285</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1379,7 +1491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7E6017-104F-43D7-803B-7E6A869158EA}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
@@ -2676,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2392CF-EBEA-424A-B0A7-A96DBE8241EA}">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3548,7 +3660,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>